<commit_message>
added 2017/2018 season data
</commit_message>
<xml_diff>
--- a/League Progress.xlsx
+++ b/League Progress.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonard.000\gitboyzorro5\FDAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonard\gitboyzorro5\FDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12540" windowHeight="7275" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12540" windowHeight="7275"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -550,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,24 +983,24 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C23" s="1">
         <v>306</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="1"/>
-        <v>0.75816993464052285</v>
+        <v>0.76470588235294112</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24">
         <f>SUM(B2:B23)</f>
-        <v>5862</v>
+        <v>5864</v>
       </c>
       <c r="C24">
         <f>SUM(C2:C23)</f>
@@ -1008,11 +1008,11 @@
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>1828</v>
+        <v>1826</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" si="1"/>
-        <v>0.76228868660598181</v>
+        <v>0.76254876462938881</v>
       </c>
     </row>
   </sheetData>
@@ -1116,7 +1116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>